<commit_message>
Updates re: reference QA/QC
</commit_message>
<xml_diff>
--- a/data/workspace.xlsx
+++ b/data/workspace.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="24360" windowHeight="15360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="workspace.csv" sheetId="1" r:id="rId1"/>
@@ -4357,11 +4357,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD570"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
+      <selection activeCell="D331" sqref="D331:D342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:56">
       <c r="A1" t="s">
@@ -34133,7 +34136,7 @@
         <v>48</v>
       </c>
       <c r="D338">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="E338" t="s">
         <v>56</v>
@@ -34201,7 +34204,7 @@
         <v>48</v>
       </c>
       <c r="D339">
-        <v>2008</v>
+        <v>2006</v>
       </c>
       <c r="E339" t="s">
         <v>56</v>
@@ -34269,7 +34272,7 @@
         <v>48</v>
       </c>
       <c r="D340">
-        <v>2009</v>
+        <v>2006</v>
       </c>
       <c r="E340" t="s">
         <v>56</v>
@@ -34337,7 +34340,7 @@
         <v>48</v>
       </c>
       <c r="D341">
-        <v>2010</v>
+        <v>2006</v>
       </c>
       <c r="E341" t="s">
         <v>56</v>
@@ -34405,7 +34408,7 @@
         <v>48</v>
       </c>
       <c r="D342">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="E342" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
fix typo re: fungicide amount
</commit_message>
<xml_diff>
--- a/data/workspace.xlsx
+++ b/data/workspace.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24680" windowHeight="15600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24700" windowHeight="15600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="workspace.csv" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6910" uniqueCount="967">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6910" uniqueCount="966">
   <si>
     <t>FID</t>
   </si>
@@ -2462,9 +2462,6 @@
   </si>
   <si>
     <t>myc fb myc + pyra</t>
-  </si>
-  <si>
-    <t>7 fb 7 = 6</t>
   </si>
   <si>
     <t>Quilt fb Folicur</t>
@@ -4333,8 +4330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AV570"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="AW1" sqref="AW1:BD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F506" workbookViewId="0">
+      <selection activeCell="Q516" sqref="Q516"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -46234,7 +46231,7 @@
         <v>72</v>
       </c>
       <c r="Q516" t="s">
-        <v>814</v>
+        <v>804</v>
       </c>
       <c r="R516" t="s">
         <v>57</v>
@@ -46290,13 +46287,13 @@
         <v>2</v>
       </c>
       <c r="L517" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="M517" t="s">
         <v>507</v>
       </c>
       <c r="N517" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="O517" t="s">
         <v>76</v>
@@ -46305,7 +46302,7 @@
         <v>72</v>
       </c>
       <c r="Q517" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="R517" t="s">
         <v>57</v>
@@ -46361,13 +46358,13 @@
         <v>2</v>
       </c>
       <c r="L518" t="s">
+        <v>817</v>
+      </c>
+      <c r="M518" t="s">
         <v>818</v>
       </c>
-      <c r="M518" t="s">
+      <c r="N518" t="s">
         <v>819</v>
-      </c>
-      <c r="N518" t="s">
-        <v>820</v>
       </c>
       <c r="O518" t="s">
         <v>76</v>
@@ -46376,7 +46373,7 @@
         <v>72</v>
       </c>
       <c r="Q518" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="R518" t="s">
         <v>57</v>
@@ -46432,13 +46429,13 @@
         <v>2</v>
       </c>
       <c r="L519" t="s">
+        <v>821</v>
+      </c>
+      <c r="M519" t="s">
         <v>822</v>
       </c>
-      <c r="M519" t="s">
+      <c r="N519" t="s">
         <v>823</v>
-      </c>
-      <c r="N519" t="s">
-        <v>824</v>
       </c>
       <c r="O519" t="s">
         <v>76</v>
@@ -46447,7 +46444,7 @@
         <v>72</v>
       </c>
       <c r="Q519" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="R519" t="s">
         <v>57</v>
@@ -46547,7 +46544,7 @@
         <v>540</v>
       </c>
       <c r="B521" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C521">
         <v>71</v>
@@ -46559,10 +46556,10 @@
         <v>447</v>
       </c>
       <c r="F521" t="s">
+        <v>826</v>
+      </c>
+      <c r="G521" t="s">
         <v>827</v>
-      </c>
-      <c r="G521" t="s">
-        <v>828</v>
       </c>
       <c r="H521">
         <v>38489</v>
@@ -46612,7 +46609,7 @@
         <v>541</v>
       </c>
       <c r="B522" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C522">
         <v>71</v>
@@ -46624,10 +46621,10 @@
         <v>447</v>
       </c>
       <c r="F522" t="s">
+        <v>826</v>
+      </c>
+      <c r="G522" t="s">
         <v>827</v>
-      </c>
-      <c r="G522" t="s">
-        <v>828</v>
       </c>
       <c r="H522">
         <v>38489</v>
@@ -46645,7 +46642,7 @@
         <v>166</v>
       </c>
       <c r="N522" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="O522" t="s">
         <v>76</v>
@@ -46677,7 +46674,7 @@
         <v>542</v>
       </c>
       <c r="B523" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C523">
         <v>71</v>
@@ -46689,10 +46686,10 @@
         <v>447</v>
       </c>
       <c r="F523" t="s">
+        <v>826</v>
+      </c>
+      <c r="G523" t="s">
         <v>827</v>
-      </c>
-      <c r="G523" t="s">
-        <v>828</v>
       </c>
       <c r="H523">
         <v>38489</v>
@@ -46704,10 +46701,10 @@
         <v>3</v>
       </c>
       <c r="L523" t="s">
+        <v>829</v>
+      </c>
+      <c r="M523" t="s">
         <v>830</v>
-      </c>
-      <c r="M523" t="s">
-        <v>831</v>
       </c>
       <c r="N523" t="s">
         <v>685</v>
@@ -46742,7 +46739,7 @@
         <v>543</v>
       </c>
       <c r="B524" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C524">
         <v>71</v>
@@ -46754,10 +46751,10 @@
         <v>447</v>
       </c>
       <c r="F524" t="s">
+        <v>826</v>
+      </c>
+      <c r="G524" t="s">
         <v>827</v>
-      </c>
-      <c r="G524" t="s">
-        <v>828</v>
       </c>
       <c r="H524">
         <v>38489</v>
@@ -46769,10 +46766,10 @@
         <v>3</v>
       </c>
       <c r="L524" t="s">
+        <v>829</v>
+      </c>
+      <c r="M524" t="s">
         <v>830</v>
-      </c>
-      <c r="M524" t="s">
-        <v>831</v>
       </c>
       <c r="N524" t="s">
         <v>685</v>
@@ -46807,7 +46804,7 @@
         <v>544</v>
       </c>
       <c r="B525" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C525">
         <v>71</v>
@@ -46819,10 +46816,10 @@
         <v>447</v>
       </c>
       <c r="F525" t="s">
+        <v>826</v>
+      </c>
+      <c r="G525" t="s">
         <v>827</v>
-      </c>
-      <c r="G525" t="s">
-        <v>828</v>
       </c>
       <c r="H525">
         <v>38489</v>
@@ -46834,10 +46831,10 @@
         <v>3</v>
       </c>
       <c r="L525" t="s">
+        <v>829</v>
+      </c>
+      <c r="M525" t="s">
         <v>830</v>
-      </c>
-      <c r="M525" t="s">
-        <v>831</v>
       </c>
       <c r="N525" t="s">
         <v>685</v>
@@ -46872,7 +46869,7 @@
         <v>545</v>
       </c>
       <c r="B526" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C526">
         <v>71</v>
@@ -46884,10 +46881,10 @@
         <v>447</v>
       </c>
       <c r="F526" t="s">
+        <v>826</v>
+      </c>
+      <c r="G526" t="s">
         <v>827</v>
-      </c>
-      <c r="G526" t="s">
-        <v>828</v>
       </c>
       <c r="H526">
         <v>38489</v>
@@ -46902,7 +46899,7 @@
         <v>501</v>
       </c>
       <c r="M526" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="N526" t="s">
         <v>659</v>
@@ -46937,7 +46934,7 @@
         <v>546</v>
       </c>
       <c r="B527" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C527">
         <v>71</v>
@@ -46949,10 +46946,10 @@
         <v>447</v>
       </c>
       <c r="F527" t="s">
+        <v>826</v>
+      </c>
+      <c r="G527" t="s">
         <v>827</v>
-      </c>
-      <c r="G527" t="s">
-        <v>828</v>
       </c>
       <c r="H527">
         <v>38489</v>
@@ -46967,7 +46964,7 @@
         <v>201</v>
       </c>
       <c r="M527" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="N527" t="s">
         <v>678</v>
@@ -46979,7 +46976,7 @@
         <v>72</v>
       </c>
       <c r="Q527" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="R527" t="s">
         <v>57</v>
@@ -47002,7 +46999,7 @@
         <v>547</v>
       </c>
       <c r="B528" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C528">
         <v>71</v>
@@ -47014,10 +47011,10 @@
         <v>447</v>
       </c>
       <c r="F528" t="s">
+        <v>826</v>
+      </c>
+      <c r="G528" t="s">
         <v>827</v>
-      </c>
-      <c r="G528" t="s">
-        <v>828</v>
       </c>
       <c r="H528">
         <v>38489</v>
@@ -47044,7 +47041,7 @@
         <v>72</v>
       </c>
       <c r="Q528" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="R528" t="s">
         <v>57</v>
@@ -47067,7 +47064,7 @@
         <v>548</v>
       </c>
       <c r="B529" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C529">
         <v>72</v>
@@ -47079,34 +47076,34 @@
         <v>307</v>
       </c>
       <c r="F529" t="s">
+        <v>836</v>
+      </c>
+      <c r="G529" t="s">
         <v>837</v>
-      </c>
-      <c r="G529" t="s">
-        <v>838</v>
       </c>
       <c r="H529">
         <v>38484</v>
       </c>
       <c r="J529" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="K529">
         <v>2</v>
       </c>
       <c r="L529" t="s">
+        <v>839</v>
+      </c>
+      <c r="M529" t="s">
         <v>840</v>
       </c>
-      <c r="M529" t="s">
+      <c r="N529" t="s">
         <v>841</v>
       </c>
-      <c r="N529" t="s">
+      <c r="O529" t="s">
         <v>842</v>
       </c>
-      <c r="O529" t="s">
-        <v>843</v>
-      </c>
       <c r="P529" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="Q529">
         <v>20</v>
@@ -47150,7 +47147,7 @@
         <v>549</v>
       </c>
       <c r="B530" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C530">
         <v>72</v>
@@ -47162,34 +47159,34 @@
         <v>307</v>
       </c>
       <c r="F530" t="s">
+        <v>836</v>
+      </c>
+      <c r="G530" t="s">
         <v>837</v>
-      </c>
-      <c r="G530" t="s">
-        <v>838</v>
       </c>
       <c r="H530">
         <v>38484</v>
       </c>
       <c r="J530" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="K530">
         <v>2</v>
       </c>
       <c r="L530" t="s">
+        <v>839</v>
+      </c>
+      <c r="M530" t="s">
         <v>840</v>
       </c>
-      <c r="M530" t="s">
+      <c r="N530" t="s">
         <v>841</v>
       </c>
-      <c r="N530" t="s">
+      <c r="O530" t="s">
         <v>842</v>
       </c>
-      <c r="O530" t="s">
-        <v>843</v>
-      </c>
       <c r="P530" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="Q530">
         <v>20</v>
@@ -47233,7 +47230,7 @@
         <v>550</v>
       </c>
       <c r="B531" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C531">
         <v>72</v>
@@ -47245,10 +47242,10 @@
         <v>307</v>
       </c>
       <c r="F531" t="s">
+        <v>836</v>
+      </c>
+      <c r="G531" t="s">
         <v>837</v>
-      </c>
-      <c r="G531" t="s">
-        <v>838</v>
       </c>
       <c r="H531">
         <v>38484</v>
@@ -47260,13 +47257,13 @@
         <v>1</v>
       </c>
       <c r="L531" t="s">
+        <v>843</v>
+      </c>
+      <c r="M531" t="s">
         <v>844</v>
       </c>
-      <c r="M531" t="s">
+      <c r="N531" t="s">
         <v>845</v>
-      </c>
-      <c r="N531" t="s">
-        <v>846</v>
       </c>
       <c r="O531" t="s">
         <v>76</v>
@@ -47275,7 +47272,7 @@
         <v>72</v>
       </c>
       <c r="Q531" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="R531" t="s">
         <v>57</v>
@@ -47316,7 +47313,7 @@
         <v>551</v>
       </c>
       <c r="B532" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C532">
         <v>72</v>
@@ -47328,10 +47325,10 @@
         <v>307</v>
       </c>
       <c r="F532" t="s">
+        <v>836</v>
+      </c>
+      <c r="G532" t="s">
         <v>837</v>
-      </c>
-      <c r="G532" t="s">
-        <v>838</v>
       </c>
       <c r="H532">
         <v>38484</v>
@@ -47399,7 +47396,7 @@
         <v>552</v>
       </c>
       <c r="B533" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C533">
         <v>72</v>
@@ -47411,10 +47408,10 @@
         <v>307</v>
       </c>
       <c r="F533" t="s">
+        <v>836</v>
+      </c>
+      <c r="G533" t="s">
         <v>837</v>
-      </c>
-      <c r="G533" t="s">
-        <v>838</v>
       </c>
       <c r="H533">
         <v>38484</v>
@@ -47429,7 +47426,7 @@
         <v>82</v>
       </c>
       <c r="M533" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="N533" t="s">
         <v>61</v>
@@ -47482,7 +47479,7 @@
         <v>553</v>
       </c>
       <c r="B534" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C534">
         <v>72</v>
@@ -47494,10 +47491,10 @@
         <v>307</v>
       </c>
       <c r="F534" t="s">
+        <v>836</v>
+      </c>
+      <c r="G534" t="s">
         <v>837</v>
-      </c>
-      <c r="G534" t="s">
-        <v>838</v>
       </c>
       <c r="H534">
         <v>38484</v>
@@ -47565,7 +47562,7 @@
         <v>554</v>
       </c>
       <c r="B535" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C535">
         <v>72</v>
@@ -47577,10 +47574,10 @@
         <v>307</v>
       </c>
       <c r="F535" t="s">
+        <v>836</v>
+      </c>
+      <c r="G535" t="s">
         <v>837</v>
-      </c>
-      <c r="G535" t="s">
-        <v>838</v>
       </c>
       <c r="H535">
         <v>38484</v>
@@ -47648,7 +47645,7 @@
         <v>555</v>
       </c>
       <c r="B536" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C536">
         <v>72</v>
@@ -47660,10 +47657,10 @@
         <v>307</v>
       </c>
       <c r="F536" t="s">
+        <v>836</v>
+      </c>
+      <c r="G536" t="s">
         <v>837</v>
-      </c>
-      <c r="G536" t="s">
-        <v>838</v>
       </c>
       <c r="H536">
         <v>38484</v>
@@ -47731,7 +47728,7 @@
         <v>556</v>
       </c>
       <c r="B537" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C537">
         <v>72</v>
@@ -47743,10 +47740,10 @@
         <v>307</v>
       </c>
       <c r="F537" t="s">
+        <v>836</v>
+      </c>
+      <c r="G537" t="s">
         <v>837</v>
-      </c>
-      <c r="G537" t="s">
-        <v>838</v>
       </c>
       <c r="H537">
         <v>38484</v>
@@ -47814,7 +47811,7 @@
         <v>557</v>
       </c>
       <c r="B538" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C538">
         <v>72</v>
@@ -47826,10 +47823,10 @@
         <v>307</v>
       </c>
       <c r="F538" t="s">
+        <v>836</v>
+      </c>
+      <c r="G538" t="s">
         <v>837</v>
-      </c>
-      <c r="G538" t="s">
-        <v>838</v>
       </c>
       <c r="H538">
         <v>38484</v>
@@ -47897,7 +47894,7 @@
         <v>558</v>
       </c>
       <c r="B539" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C539">
         <v>72</v>
@@ -47909,10 +47906,10 @@
         <v>307</v>
       </c>
       <c r="F539" t="s">
+        <v>836</v>
+      </c>
+      <c r="G539" t="s">
         <v>837</v>
-      </c>
-      <c r="G539" t="s">
-        <v>838</v>
       </c>
       <c r="H539">
         <v>38484</v>
@@ -47980,7 +47977,7 @@
         <v>559</v>
       </c>
       <c r="B540" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C540">
         <v>72</v>
@@ -47992,10 +47989,10 @@
         <v>307</v>
       </c>
       <c r="F540" t="s">
+        <v>836</v>
+      </c>
+      <c r="G540" t="s">
         <v>837</v>
-      </c>
-      <c r="G540" t="s">
-        <v>838</v>
       </c>
       <c r="H540">
         <v>38484</v>
@@ -48039,7 +48036,7 @@
         <v>560</v>
       </c>
       <c r="B541" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C541">
         <v>72</v>
@@ -48051,10 +48048,10 @@
         <v>307</v>
       </c>
       <c r="F541" t="s">
+        <v>836</v>
+      </c>
+      <c r="G541" t="s">
         <v>837</v>
-      </c>
-      <c r="G541" t="s">
-        <v>838</v>
       </c>
       <c r="H541">
         <v>38484</v>
@@ -48069,7 +48066,7 @@
         <v>82</v>
       </c>
       <c r="M541" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="N541" t="s">
         <v>61</v>
@@ -48098,7 +48095,7 @@
         <v>561</v>
       </c>
       <c r="B542" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C542">
         <v>72</v>
@@ -48110,10 +48107,10 @@
         <v>307</v>
       </c>
       <c r="F542" t="s">
+        <v>836</v>
+      </c>
+      <c r="G542" t="s">
         <v>837</v>
-      </c>
-      <c r="G542" t="s">
-        <v>838</v>
       </c>
       <c r="H542">
         <v>38484</v>
@@ -48157,7 +48154,7 @@
         <v>562</v>
       </c>
       <c r="B543" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C543">
         <v>72</v>
@@ -48169,10 +48166,10 @@
         <v>307</v>
       </c>
       <c r="F543" t="s">
+        <v>836</v>
+      </c>
+      <c r="G543" t="s">
         <v>837</v>
-      </c>
-      <c r="G543" t="s">
-        <v>838</v>
       </c>
       <c r="H543">
         <v>38484</v>
@@ -48190,7 +48187,7 @@
         <v>166</v>
       </c>
       <c r="N543" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="O543" t="s">
         <v>76</v>
@@ -48216,7 +48213,7 @@
         <v>563</v>
       </c>
       <c r="B544" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C544">
         <v>73</v>
@@ -48228,10 +48225,10 @@
         <v>307</v>
       </c>
       <c r="F544" t="s">
+        <v>836</v>
+      </c>
+      <c r="G544" t="s">
         <v>837</v>
-      </c>
-      <c r="G544" t="s">
-        <v>838</v>
       </c>
       <c r="H544">
         <v>38489</v>
@@ -48246,7 +48243,7 @@
         <v>82</v>
       </c>
       <c r="M544" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="N544" t="s">
         <v>61</v>
@@ -48299,7 +48296,7 @@
         <v>564</v>
       </c>
       <c r="B545" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C545">
         <v>73</v>
@@ -48311,10 +48308,10 @@
         <v>307</v>
       </c>
       <c r="F545" t="s">
+        <v>836</v>
+      </c>
+      <c r="G545" t="s">
         <v>837</v>
-      </c>
-      <c r="G545" t="s">
-        <v>838</v>
       </c>
       <c r="H545">
         <v>38489</v>
@@ -48382,7 +48379,7 @@
         <v>565</v>
       </c>
       <c r="B546" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C546">
         <v>73</v>
@@ -48394,10 +48391,10 @@
         <v>307</v>
       </c>
       <c r="F546" t="s">
+        <v>836</v>
+      </c>
+      <c r="G546" t="s">
         <v>837</v>
-      </c>
-      <c r="G546" t="s">
-        <v>838</v>
       </c>
       <c r="H546">
         <v>38489</v>
@@ -48465,7 +48462,7 @@
         <v>566</v>
       </c>
       <c r="B547" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C547">
         <v>73</v>
@@ -48477,10 +48474,10 @@
         <v>307</v>
       </c>
       <c r="F547" t="s">
+        <v>836</v>
+      </c>
+      <c r="G547" t="s">
         <v>837</v>
-      </c>
-      <c r="G547" t="s">
-        <v>838</v>
       </c>
       <c r="H547">
         <v>38489</v>
@@ -48495,7 +48492,7 @@
         <v>82</v>
       </c>
       <c r="M547" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="N547" t="s">
         <v>61</v>
@@ -48548,7 +48545,7 @@
         <v>567</v>
       </c>
       <c r="B548" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C548">
         <v>73</v>
@@ -48560,10 +48557,10 @@
         <v>307</v>
       </c>
       <c r="F548" t="s">
+        <v>836</v>
+      </c>
+      <c r="G548" t="s">
         <v>837</v>
-      </c>
-      <c r="G548" t="s">
-        <v>838</v>
       </c>
       <c r="H548">
         <v>38489</v>
@@ -48631,7 +48628,7 @@
         <v>568</v>
       </c>
       <c r="B549" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C549">
         <v>73</v>
@@ -48643,10 +48640,10 @@
         <v>307</v>
       </c>
       <c r="F549" t="s">
+        <v>836</v>
+      </c>
+      <c r="G549" t="s">
         <v>837</v>
-      </c>
-      <c r="G549" t="s">
-        <v>838</v>
       </c>
       <c r="H549">
         <v>38489</v>
@@ -48714,7 +48711,7 @@
         <v>569</v>
       </c>
       <c r="B550" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C550">
         <v>73</v>
@@ -48726,10 +48723,10 @@
         <v>307</v>
       </c>
       <c r="F550" t="s">
+        <v>836</v>
+      </c>
+      <c r="G550" t="s">
         <v>837</v>
-      </c>
-      <c r="G550" t="s">
-        <v>838</v>
       </c>
       <c r="H550">
         <v>38489</v>
@@ -48747,7 +48744,7 @@
         <v>166</v>
       </c>
       <c r="N550" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="O550" t="s">
         <v>76</v>
@@ -48797,7 +48794,7 @@
         <v>570</v>
       </c>
       <c r="B551" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C551">
         <v>73</v>
@@ -48809,10 +48806,10 @@
         <v>307</v>
       </c>
       <c r="F551" t="s">
+        <v>836</v>
+      </c>
+      <c r="G551" t="s">
         <v>837</v>
-      </c>
-      <c r="G551" t="s">
-        <v>838</v>
       </c>
       <c r="H551">
         <v>38489</v>
@@ -48880,7 +48877,7 @@
         <v>571</v>
       </c>
       <c r="B552" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C552">
         <v>73</v>
@@ -48892,10 +48889,10 @@
         <v>307</v>
       </c>
       <c r="F552" t="s">
+        <v>836</v>
+      </c>
+      <c r="G552" t="s">
         <v>837</v>
-      </c>
-      <c r="G552" t="s">
-        <v>838</v>
       </c>
       <c r="H552">
         <v>38489</v>
@@ -48910,7 +48907,7 @@
         <v>82</v>
       </c>
       <c r="M552" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="N552" t="s">
         <v>61</v>
@@ -48963,7 +48960,7 @@
         <v>572</v>
       </c>
       <c r="B553" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C553">
         <v>73</v>
@@ -48975,10 +48972,10 @@
         <v>307</v>
       </c>
       <c r="F553" t="s">
+        <v>836</v>
+      </c>
+      <c r="G553" t="s">
         <v>837</v>
-      </c>
-      <c r="G553" t="s">
-        <v>838</v>
       </c>
       <c r="H553">
         <v>38489</v>
@@ -49046,7 +49043,7 @@
         <v>573</v>
       </c>
       <c r="B554" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C554">
         <v>73</v>
@@ -49058,10 +49055,10 @@
         <v>307</v>
       </c>
       <c r="F554" t="s">
+        <v>836</v>
+      </c>
+      <c r="G554" t="s">
         <v>837</v>
-      </c>
-      <c r="G554" t="s">
-        <v>838</v>
       </c>
       <c r="H554">
         <v>38489</v>
@@ -49129,7 +49126,7 @@
         <v>574</v>
       </c>
       <c r="B555" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C555">
         <v>73</v>
@@ -49141,10 +49138,10 @@
         <v>307</v>
       </c>
       <c r="F555" t="s">
+        <v>836</v>
+      </c>
+      <c r="G555" t="s">
         <v>837</v>
-      </c>
-      <c r="G555" t="s">
-        <v>838</v>
       </c>
       <c r="H555">
         <v>38489</v>
@@ -49188,7 +49185,7 @@
         <v>575</v>
       </c>
       <c r="B556" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C556">
         <v>73</v>
@@ -49200,10 +49197,10 @@
         <v>307</v>
       </c>
       <c r="F556" t="s">
+        <v>836</v>
+      </c>
+      <c r="G556" t="s">
         <v>837</v>
-      </c>
-      <c r="G556" t="s">
-        <v>838</v>
       </c>
       <c r="H556">
         <v>38489</v>
@@ -49218,7 +49215,7 @@
         <v>82</v>
       </c>
       <c r="M556" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="N556" t="s">
         <v>61</v>
@@ -49247,7 +49244,7 @@
         <v>576</v>
       </c>
       <c r="B557" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C557">
         <v>73</v>
@@ -49259,10 +49256,10 @@
         <v>307</v>
       </c>
       <c r="F557" t="s">
+        <v>836</v>
+      </c>
+      <c r="G557" t="s">
         <v>837</v>
-      </c>
-      <c r="G557" t="s">
-        <v>838</v>
       </c>
       <c r="H557">
         <v>38489</v>
@@ -49306,7 +49303,7 @@
         <v>577</v>
       </c>
       <c r="B558" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C558">
         <v>73</v>
@@ -49318,10 +49315,10 @@
         <v>307</v>
       </c>
       <c r="F558" t="s">
+        <v>836</v>
+      </c>
+      <c r="G558" t="s">
         <v>837</v>
-      </c>
-      <c r="G558" t="s">
-        <v>838</v>
       </c>
       <c r="H558">
         <v>38489</v>
@@ -49336,7 +49333,7 @@
         <v>82</v>
       </c>
       <c r="M558" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="N558" t="s">
         <v>61</v>
@@ -49365,7 +49362,7 @@
         <v>578</v>
       </c>
       <c r="B559" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C559">
         <v>74</v>
@@ -49386,7 +49383,7 @@
         <v>38869</v>
       </c>
       <c r="J559" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="K559">
         <v>2</v>
@@ -49448,7 +49445,7 @@
         <v>579</v>
       </c>
       <c r="B560" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C560">
         <v>74</v>
@@ -49499,7 +49496,7 @@
         <v>5</v>
       </c>
       <c r="T560" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="Y560">
         <v>6</v>
@@ -49531,7 +49528,7 @@
         <v>580</v>
       </c>
       <c r="B561" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C561">
         <v>74</v>
@@ -49552,7 +49549,7 @@
         <v>38871</v>
       </c>
       <c r="J561" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="K561">
         <v>2</v>
@@ -49582,7 +49579,7 @@
         <v>6</v>
       </c>
       <c r="T561" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="Y561">
         <v>6</v>
@@ -49614,7 +49611,7 @@
         <v>581</v>
       </c>
       <c r="B562" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C562">
         <v>74</v>
@@ -49635,19 +49632,19 @@
         <v>38872</v>
       </c>
       <c r="J562" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="K562">
         <v>2</v>
       </c>
       <c r="L562" t="s">
+        <v>855</v>
+      </c>
+      <c r="M562" t="s">
         <v>856</v>
       </c>
-      <c r="M562" t="s">
+      <c r="N562" t="s">
         <v>857</v>
-      </c>
-      <c r="N562" t="s">
-        <v>858</v>
       </c>
       <c r="O562" t="s">
         <v>76</v>
@@ -49665,7 +49662,7 @@
         <v>7</v>
       </c>
       <c r="T562" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="Y562">
         <v>0</v>
@@ -49697,7 +49694,7 @@
         <v>582</v>
       </c>
       <c r="B563" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C563">
         <v>74</v>
@@ -49718,7 +49715,7 @@
         <v>38873</v>
       </c>
       <c r="J563" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="K563">
         <v>2</v>
@@ -49727,7 +49724,7 @@
         <v>798</v>
       </c>
       <c r="M563" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="N563" t="s">
         <v>800</v>
@@ -49748,7 +49745,7 @@
         <v>8</v>
       </c>
       <c r="T563" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="Y563">
         <v>2</v>
@@ -49780,7 +49777,7 @@
         <v>583</v>
       </c>
       <c r="B564" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C564">
         <v>74</v>
@@ -49801,19 +49798,19 @@
         <v>38874</v>
       </c>
       <c r="J564" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="K564">
         <v>2</v>
       </c>
       <c r="L564" t="s">
+        <v>863</v>
+      </c>
+      <c r="M564" t="s">
         <v>864</v>
       </c>
-      <c r="M564" t="s">
+      <c r="N564" t="s">
         <v>865</v>
-      </c>
-      <c r="N564" t="s">
-        <v>866</v>
       </c>
       <c r="O564" t="s">
         <v>76</v>
@@ -49831,7 +49828,7 @@
         <v>9</v>
       </c>
       <c r="T564" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="Y564">
         <v>2</v>
@@ -49863,7 +49860,7 @@
         <v>584</v>
       </c>
       <c r="B565" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C565">
         <v>74</v>
@@ -49884,7 +49881,7 @@
         <v>38875</v>
       </c>
       <c r="J565" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="K565">
         <v>2</v>
@@ -49896,7 +49893,7 @@
         <v>517</v>
       </c>
       <c r="N565" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="O565" t="s">
         <v>76</v>
@@ -49914,7 +49911,7 @@
         <v>10</v>
       </c>
       <c r="T565" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="Y565">
         <v>1</v>
@@ -49946,7 +49943,7 @@
         <v>585</v>
       </c>
       <c r="B566" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C566">
         <v>74</v>
@@ -49967,7 +49964,7 @@
         <v>38876</v>
       </c>
       <c r="J566" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="K566">
         <v>2</v>
@@ -49976,10 +49973,10 @@
         <v>807</v>
       </c>
       <c r="M566" t="s">
+        <v>871</v>
+      </c>
+      <c r="N566" t="s">
         <v>872</v>
-      </c>
-      <c r="N566" t="s">
-        <v>873</v>
       </c>
       <c r="O566" t="s">
         <v>76</v>
@@ -49997,7 +49994,7 @@
         <v>11</v>
       </c>
       <c r="T566" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="Y566">
         <v>1</v>
@@ -50029,7 +50026,7 @@
         <v>586</v>
       </c>
       <c r="B567" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C567">
         <v>74</v>
@@ -50050,19 +50047,19 @@
         <v>38877</v>
       </c>
       <c r="J567" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="K567">
         <v>2</v>
       </c>
       <c r="L567" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="M567" t="s">
+        <v>875</v>
+      </c>
+      <c r="N567" t="s">
         <v>876</v>
-      </c>
-      <c r="N567" t="s">
-        <v>877</v>
       </c>
       <c r="O567" t="s">
         <v>76</v>
@@ -50071,7 +50068,7 @@
         <v>72</v>
       </c>
       <c r="Q567" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="R567" t="s">
         <v>57</v>
@@ -50080,7 +50077,7 @@
         <v>12</v>
       </c>
       <c r="T567" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="Y567">
         <v>6</v>
@@ -50112,7 +50109,7 @@
         <v>587</v>
       </c>
       <c r="B568" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C568">
         <v>74</v>
@@ -50133,19 +50130,19 @@
         <v>38878</v>
       </c>
       <c r="J568" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="K568">
         <v>2</v>
       </c>
       <c r="L568" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="M568" t="s">
+        <v>879</v>
+      </c>
+      <c r="N568" t="s">
         <v>880</v>
-      </c>
-      <c r="N568" t="s">
-        <v>881</v>
       </c>
       <c r="O568" t="s">
         <v>76</v>
@@ -50154,7 +50151,7 @@
         <v>72</v>
       </c>
       <c r="Q568" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="R568" t="s">
         <v>57</v>
@@ -50195,7 +50192,7 @@
         <v>588</v>
       </c>
       <c r="B569" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C569">
         <v>74</v>
@@ -50216,19 +50213,19 @@
         <v>38879</v>
       </c>
       <c r="J569" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="K569">
         <v>2</v>
       </c>
       <c r="L569" t="s">
+        <v>882</v>
+      </c>
+      <c r="M569" t="s">
         <v>883</v>
       </c>
-      <c r="M569" t="s">
+      <c r="N569" t="s">
         <v>884</v>
-      </c>
-      <c r="N569" t="s">
-        <v>885</v>
       </c>
       <c r="O569" t="s">
         <v>76</v>
@@ -50237,7 +50234,7 @@
         <v>72</v>
       </c>
       <c r="Q569" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="R569" t="s">
         <v>57</v>
@@ -50246,7 +50243,7 @@
         <v>14</v>
       </c>
       <c r="T569" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="Y569">
         <v>2</v>
@@ -50278,7 +50275,7 @@
         <v>589</v>
       </c>
       <c r="B570" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C570">
         <v>74</v>
@@ -50299,19 +50296,19 @@
         <v>38880</v>
       </c>
       <c r="J570" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="K570">
         <v>2</v>
       </c>
       <c r="L570" t="s">
+        <v>887</v>
+      </c>
+      <c r="M570" t="s">
         <v>888</v>
       </c>
-      <c r="M570" t="s">
+      <c r="N570" t="s">
         <v>889</v>
-      </c>
-      <c r="N570" t="s">
-        <v>890</v>
       </c>
       <c r="O570" t="s">
         <v>76</v>
@@ -50329,7 +50326,7 @@
         <v>15</v>
       </c>
       <c r="T570" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="Y570">
         <v>2</v>
@@ -50381,381 +50378,381 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="2" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="2" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="2" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="2" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="2" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="2" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="4" t="s">
+        <v>900</v>
+      </c>
+      <c r="B10" t="s">
         <v>901</v>
-      </c>
-      <c r="B10" t="s">
-        <v>902</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="2" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="2" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="2" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="2" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="5" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="18" spans="1:1">
       <c r="A18" s="5" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="19" spans="1:1">
       <c r="A19" s="5" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="6" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="21" spans="1:1">
       <c r="A21" s="6" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="5" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="23" spans="1:1">
       <c r="A23" s="5" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="24" spans="1:1">
       <c r="A24" s="5" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="5" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="26" spans="1:1">
       <c r="A26" s="5" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="27" spans="1:1">
       <c r="A27" s="5" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="5" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="29" spans="1:1">
       <c r="A29" s="5" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="30" spans="1:1">
       <c r="A30" s="5" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="31" spans="1:1">
       <c r="A31" s="5" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="32" spans="1:1">
       <c r="A32" s="5" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" s="5" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" s="5" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" s="5" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="5" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" s="5" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="5" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" s="5" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="5" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="41" spans="1:1">
       <c r="A41" s="5" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="5" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="5" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="5" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="45" spans="1:1">
       <c r="A45" s="5" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="7" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="47" spans="1:1">
       <c r="A47" s="5" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="5" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="8" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="9" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B56" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="9" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B57" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="9" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="10" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="10" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="8" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="10" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="65" spans="1:1">
       <c r="A65" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="66" spans="1:1" s="10" customFormat="1">
       <c r="A66" s="10" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="67" spans="1:1" s="10" customFormat="1">
       <c r="A67" s="10" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="68" spans="1:1" s="10" customFormat="1">
       <c r="A68" s="10" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="69" spans="1:1" s="10" customFormat="1">
       <c r="A69" s="10" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="70" spans="1:1" s="10" customFormat="1">
       <c r="A70" s="10" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="71" spans="1:1" s="10" customFormat="1">
       <c r="A71" s="10" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="72" spans="1:1" s="10" customFormat="1">
       <c r="A72" s="10" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="73" spans="1:1">
       <c r="A73" s="10" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="74" spans="1:1" s="10" customFormat="1">
       <c r="A74" s="10" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
   </sheetData>

</xml_diff>